<commit_message>
begin cleaning combined data
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bellamullen/Documents/GITHUB/critcher2013_1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698CCDBF-1C84-B74B-A221-7AC66A313090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A4009F-7CAA-4D4B-9E3F-11BE72555660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{E9DEE37D-E88E-B24C-A45F-3AAD6737441E}"/>
   </bookViews>
@@ -101,9 +101,6 @@
     <t>(Milliseconds)</t>
   </si>
   <si>
-    <t>Identifies whether the question pertains to "Justin" or "Nate".</t>
-  </si>
-  <si>
     <t>4-25</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>Reverse-coded responses from 6 questions (9, 10, 13, 19, 20, 23) for consistency on the rating scale.</t>
+  </si>
+  <si>
+    <t>Identifies whether the question pertains to "Justin" (fast) or "Nate" (slow).</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,7 +573,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>17</v>
@@ -604,7 +604,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -615,13 +615,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -629,10 +629,10 @@
         <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -643,10 +643,10 @@
         <v>14</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -660,7 +660,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>